<commit_message>
Guardar cambios: solicitud de usuario
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -31,58 +31,79 @@
     <t>tramite</t>
   </si>
   <si>
+    <t>entidad</t>
+  </si>
+  <si>
+    <t>monto_alcanza</t>
+  </si>
+  <si>
+    <t>plazo</t>
+  </si>
+  <si>
+    <t>estado_civil</t>
+  </si>
+  <si>
+    <t>tipo_vivienda</t>
+  </si>
+  <si>
+    <t>tiempo_pensionado</t>
+  </si>
+  <si>
+    <t>contrasena_sipre</t>
+  </si>
+  <si>
+    <t>ref1_nombre</t>
+  </si>
+  <si>
+    <t>ref1_telefono</t>
+  </si>
+  <si>
+    <t>ref1_parentesco</t>
+  </si>
+  <si>
+    <t>ref2_nombre</t>
+  </si>
+  <si>
+    <t>ref2_telefono</t>
+  </si>
+  <si>
+    <t>ref2_parentesco</t>
+  </si>
+  <si>
+    <t>asesor</t>
+  </si>
+  <si>
+    <t>asesor_venta</t>
+  </si>
+  <si>
+    <t>fuente</t>
+  </si>
+  <si>
+    <t>fuente_base_nombre</t>
+  </si>
+  <si>
     <t>fecha_ingreso</t>
   </si>
   <si>
+    <t>fecha_dispersion</t>
+  </si>
+  <si>
     <t>fecha_proximo</t>
   </si>
   <si>
-    <t>cliente_potencial</t>
-  </si>
-  <si>
-    <t>cliente_no</t>
-  </si>
-  <si>
-    <t>buzon</t>
-  </si>
-  <si>
-    <t>asesor_venta</t>
-  </si>
-  <si>
-    <t>asesor</t>
-  </si>
-  <si>
     <t>estatus</t>
   </si>
   <si>
-    <t>monto_propuesta</t>
-  </si>
-  <si>
-    <t>monto_final</t>
-  </si>
-  <si>
-    <t>segundo_estatus</t>
-  </si>
-  <si>
     <t>observaciones</t>
   </si>
   <si>
     <t>score</t>
   </si>
   <si>
-    <t>analista</t>
-  </si>
-  <si>
-    <t>fuente</t>
-  </si>
-  <si>
     <t>sucursal</t>
   </si>
   <si>
-    <t>fecha_dispersion</t>
-  </si>
-  <si>
-    <t>C-1000</t>
+    <t>C1000</t>
   </si>
   <si>
     <t>Cliente Integración</t>
@@ -94,28 +115,22 @@
     <t>integracion@test.com</t>
   </si>
   <si>
+    <t>Asesor Test</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>2025-11-27</t>
   </si>
   <si>
-    <t>Asesor Test</t>
-  </si>
-  <si>
     <t>PENDIENTE CLIENTE</t>
   </si>
   <si>
-    <t>50000</t>
-  </si>
-  <si>
     <t>Cliente creado por test de integración</t>
   </si>
   <si>
     <t>700</t>
-  </si>
-  <si>
-    <t>Test Analyst</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
   <si>
     <t>TOXQUI</t>
@@ -476,13 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,46 +564,61 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" t="s">
         <v>33</v>
       </c>
       <c r="U2" t="s">
         <v>34</v>
+      </c>
+      <c r="W2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove all traces of segundo_estatus; make catalog I/O robust; fix historial cache; update tests and .gitignore
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -22,118 +22,82 @@
     <t>nombre</t>
   </si>
   <si>
+    <t>sucursal</t>
+  </si>
+  <si>
+    <t>asesor</t>
+  </si>
+  <si>
+    <t>fecha_ingreso</t>
+  </si>
+  <si>
+    <t>fecha_dispersion</t>
+  </si>
+  <si>
+    <t>estatus</t>
+  </si>
+  <si>
+    <t>monto_propuesta</t>
+  </si>
+  <si>
+    <t>monto_final</t>
+  </si>
+  <si>
+    <t>observaciones</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
     <t>telefono</t>
   </si>
   <si>
     <t>correo</t>
   </si>
   <si>
-    <t>tramite</t>
-  </si>
-  <si>
-    <t>entidad</t>
-  </si>
-  <si>
-    <t>monto_alcanza</t>
-  </si>
-  <si>
-    <t>plazo</t>
-  </si>
-  <si>
-    <t>estado_civil</t>
-  </si>
-  <si>
-    <t>tipo_vivienda</t>
-  </si>
-  <si>
-    <t>tiempo_pensionado</t>
-  </si>
-  <si>
-    <t>contrasena_sipre</t>
-  </si>
-  <si>
-    <t>ref1_nombre</t>
-  </si>
-  <si>
-    <t>ref1_telefono</t>
-  </si>
-  <si>
-    <t>ref1_parentesco</t>
-  </si>
-  <si>
-    <t>ref2_nombre</t>
-  </si>
-  <si>
-    <t>ref2_telefono</t>
-  </si>
-  <si>
-    <t>ref2_parentesco</t>
-  </si>
-  <si>
-    <t>asesor</t>
-  </si>
-  <si>
-    <t>asesor_venta</t>
+    <t>analista</t>
   </si>
   <si>
     <t>fuente</t>
   </si>
   <si>
-    <t>fuente_base_nombre</t>
-  </si>
-  <si>
-    <t>fecha_ingreso</t>
-  </si>
-  <si>
-    <t>fecha_dispersion</t>
-  </si>
-  <si>
-    <t>fecha_proximo</t>
-  </si>
-  <si>
-    <t>estatus</t>
-  </si>
-  <si>
-    <t>observaciones</t>
-  </si>
-  <si>
-    <t>score</t>
-  </si>
-  <si>
-    <t>sucursal</t>
-  </si>
-  <si>
     <t>C1000</t>
   </si>
   <si>
     <t>Cliente Integración</t>
   </si>
   <si>
+    <t>TOXQUI</t>
+  </si>
+  <si>
+    <t>Asesor Test</t>
+  </si>
+  <si>
+    <t>2025-12-10</t>
+  </si>
+  <si>
+    <t>PENDIENTE CLIENTE</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>Cliente creado por test de integración</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
     <t>5551234567</t>
   </si>
   <si>
     <t>integracion@test.com</t>
   </si>
   <si>
-    <t>Asesor Test</t>
+    <t>Test Analyst</t>
   </si>
   <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>2025-11-27</t>
-  </si>
-  <si>
-    <t>PENDIENTE CLIENTE</t>
-  </si>
-  <si>
-    <t>Cliente creado por test de integración</t>
-  </si>
-  <si>
-    <t>700</t>
-  </si>
-  <si>
-    <t>TOXQUI</t>
   </si>
 </sst>
 </file>
@@ -491,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,82 +507,46 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="O2" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 'producto' to client form; remove 'Analista' from alta; other small fixes
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -61,6 +61,9 @@
     <t>fuente</t>
   </si>
   <si>
+    <t>producto</t>
+  </si>
+  <si>
     <t>C1000</t>
   </si>
   <si>
@@ -73,7 +76,7 @@
     <t>Asesor Test</t>
   </si>
   <si>
-    <t>2025-12-10</t>
+    <t>2025-12-11</t>
   </si>
   <si>
     <t>PENDIENTE CLIENTE</t>
@@ -455,13 +458,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,46 +510,49 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Client form: enforce parental relationship options; limit Fuente to LUZWARE/LEADS/SEGUIMIENTO with base-name for LUZWARE; add Usuario Cipre & Contraseña; store fuente_base; expose fields in editor
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -61,7 +61,52 @@
     <t>fuente</t>
   </si>
   <si>
+    <t>tipo_tramite</t>
+  </si>
+  <si>
+    <t>capacidad</t>
+  </si>
+  <si>
+    <t>plazo</t>
+  </si>
+  <si>
+    <t>estado_civil</t>
+  </si>
+  <si>
+    <t>tipo_vivienda</t>
+  </si>
+  <si>
+    <t>ref1_nombre</t>
+  </si>
+  <si>
+    <t>ref1_telefono</t>
+  </si>
+  <si>
+    <t>ref1_parentesco</t>
+  </si>
+  <si>
+    <t>ref2_nombre</t>
+  </si>
+  <si>
+    <t>ref2_telefono</t>
+  </si>
+  <si>
+    <t>ref2_parentesco</t>
+  </si>
+  <si>
+    <t>antiguedad_cuenta</t>
+  </si>
+  <si>
     <t>producto</t>
+  </si>
+  <si>
+    <t>fuente_base</t>
+  </si>
+  <si>
+    <t>usuario_cipre</t>
+  </si>
+  <si>
+    <t>contrasena</t>
   </si>
   <si>
     <t>C1000</t>
@@ -458,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,46 +558,91 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>